<commit_message>
duplicate valencia scenarios for Groningen and Belfast Add pre-emptive code for when feedback ratings amd feedback text is available to show Make sure that buttons are disabled at game start
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Preston/AllLancashireScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Preston/AllLancashireScenarios.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="133">
   <si>
     <t>Missing Person</t>
   </si>
@@ -401,6 +401,24 @@
   <si>
     <t>Scenario_12</t>
   </si>
+  <si>
+    <t>Wait Feedback Rating</t>
+  </si>
+  <si>
+    <t>Wait Feedback</t>
+  </si>
+  <si>
+    <t>Officer Feedback Rating</t>
+  </si>
+  <si>
+    <t>Officer Feedback</t>
+  </si>
+  <si>
+    <t>Citizen Feedback Rating</t>
+  </si>
+  <si>
+    <t>Citizen Feedback</t>
+  </si>
 </sst>
 </file>
 
@@ -754,9 +772,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="Q88" sqref="Q88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -836,6 +854,24 @@
       <c r="K2" t="s">
         <v>125</v>
       </c>
+      <c r="L2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
@@ -871,12 +907,24 @@
       <c r="K3" s="2">
         <v>0</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="L3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>-1</v>
+      </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -921,12 +969,24 @@
       <c r="K4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+      <c r="L4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>-1</v>
+      </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -971,12 +1031,24 @@
       <c r="K5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="L5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>-1</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -1021,12 +1093,24 @@
       <c r="K6" s="2">
         <v>4</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="L6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>-1</v>
+      </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -1071,12 +1155,24 @@
       <c r="K7" s="2">
         <v>4</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="L7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>-1</v>
+      </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -1121,12 +1217,24 @@
       <c r="K8" s="2">
         <v>-6</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="L8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>-1</v>
+      </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -1171,12 +1279,24 @@
       <c r="K9" s="3">
         <v>0</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="L9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>-1</v>
+      </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -1221,12 +1341,24 @@
       <c r="K10" s="3">
         <v>0</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="L10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>-1</v>
+      </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -1271,12 +1403,24 @@
       <c r="K11" s="3">
         <v>0</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="L11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>-1</v>
+      </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -1321,12 +1465,24 @@
       <c r="K12" s="3">
         <v>0</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="L12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>-1</v>
+      </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -1371,12 +1527,24 @@
       <c r="K13" s="3">
         <v>0</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="L13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>-1</v>
+      </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -1421,12 +1589,24 @@
       <c r="K14" s="3">
         <v>0</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
+      <c r="L14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>-1</v>
+      </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -1471,12 +1651,24 @@
       <c r="K15" s="3">
         <v>1</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="L15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>-1</v>
+      </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -1521,12 +1713,24 @@
       <c r="K16" s="3">
         <v>1</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="L16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>-1</v>
+      </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -1571,12 +1775,24 @@
       <c r="K17" s="3">
         <v>2</v>
       </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="L17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>-1</v>
+      </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -1621,12 +1837,24 @@
       <c r="K18" s="3">
         <v>2</v>
       </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
+      <c r="L18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>-1</v>
+      </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -1671,12 +1899,24 @@
       <c r="K19" s="3">
         <v>-4</v>
       </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="L19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>-1</v>
+      </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -1721,12 +1961,24 @@
       <c r="K20" s="3">
         <v>4</v>
       </c>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="L20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>-1</v>
+      </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -1771,12 +2023,24 @@
       <c r="K21" s="3">
         <v>4</v>
       </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
+      <c r="L21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>-1</v>
+      </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -1821,12 +2085,24 @@
       <c r="K22" s="3">
         <v>5</v>
       </c>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+      <c r="L22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>-1</v>
+      </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -1871,12 +2147,24 @@
       <c r="K23" s="3">
         <v>0</v>
       </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="L23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>-1</v>
+      </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -1921,12 +2209,24 @@
       <c r="K24" s="3">
         <v>-2</v>
       </c>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="L24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>-1</v>
+      </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -1971,12 +2271,24 @@
       <c r="K25" s="3">
         <v>0</v>
       </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+      <c r="L25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>-1</v>
+      </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
@@ -2021,12 +2333,24 @@
       <c r="K26" s="3">
         <v>1</v>
       </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="L26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>-1</v>
+      </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -2071,12 +2395,24 @@
       <c r="K27" s="3">
         <v>0</v>
       </c>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
+      <c r="L27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>-1</v>
+      </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
@@ -2121,12 +2457,24 @@
       <c r="K28" s="3">
         <v>3</v>
       </c>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
+      <c r="L28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>-1</v>
+      </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
@@ -2171,12 +2519,24 @@
       <c r="K29" s="3">
         <v>0</v>
       </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
+      <c r="L29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>-1</v>
+      </c>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
@@ -2221,12 +2581,24 @@
       <c r="K30" s="3">
         <v>1</v>
       </c>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
+      <c r="L30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>-1</v>
+      </c>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
@@ -2271,12 +2643,24 @@
       <c r="K31" s="3">
         <v>1</v>
       </c>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
+      <c r="L31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>-1</v>
+      </c>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
@@ -2321,12 +2705,24 @@
       <c r="K32" s="3">
         <v>-1</v>
       </c>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
+      <c r="L32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>-1</v>
+      </c>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
@@ -2371,12 +2767,24 @@
       <c r="K33" s="3">
         <v>-2</v>
       </c>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
+      <c r="L33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>-1</v>
+      </c>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
@@ -2421,12 +2829,24 @@
       <c r="K34" s="3">
         <v>0</v>
       </c>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
+      <c r="L34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>-1</v>
+      </c>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
@@ -2471,12 +2891,24 @@
       <c r="K35" s="3">
         <v>-1</v>
       </c>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
+      <c r="L35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>-1</v>
+      </c>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
@@ -2521,12 +2953,24 @@
       <c r="K36" s="3">
         <v>0</v>
       </c>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
+      <c r="L36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>-1</v>
+      </c>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
@@ -2571,12 +3015,24 @@
       <c r="K37" s="3">
         <v>2</v>
       </c>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
+      <c r="L37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>-1</v>
+      </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
@@ -2621,12 +3077,24 @@
       <c r="K38" s="3">
         <v>-1</v>
       </c>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
+      <c r="L38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>-1</v>
+      </c>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
@@ -2671,12 +3139,24 @@
       <c r="K39" s="3">
         <v>0</v>
       </c>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
+      <c r="L39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>-1</v>
+      </c>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
@@ -2721,12 +3201,24 @@
       <c r="K40" s="3">
         <v>2</v>
       </c>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
+      <c r="L40" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M40" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N40" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O40" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P40" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>-1</v>
+      </c>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -2771,12 +3263,24 @@
       <c r="K41" s="3">
         <v>0</v>
       </c>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
+      <c r="L41" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M41" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N41" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O41" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P41" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>-1</v>
+      </c>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
@@ -2821,12 +3325,24 @@
       <c r="K42" s="3">
         <v>0</v>
       </c>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
+      <c r="L42" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M42" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N42" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O42" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P42" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>-1</v>
+      </c>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
@@ -2871,12 +3387,24 @@
       <c r="K43" s="3">
         <v>-4</v>
       </c>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
+      <c r="L43" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M43" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N43" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O43" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P43" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>-1</v>
+      </c>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
@@ -2921,12 +3449,24 @@
       <c r="K44" s="3">
         <v>0</v>
       </c>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
+      <c r="L44" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M44" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N44" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O44" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P44" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>-1</v>
+      </c>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
@@ -2971,12 +3511,24 @@
       <c r="K45" s="3">
         <v>4</v>
       </c>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
+      <c r="L45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>-1</v>
+      </c>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
@@ -3021,12 +3573,24 @@
       <c r="K46" s="3">
         <v>0</v>
       </c>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
+      <c r="L46" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M46" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N46" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O46" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P46" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>-1</v>
+      </c>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
@@ -3071,12 +3635,24 @@
       <c r="K47" s="3">
         <v>2</v>
       </c>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
+      <c r="L47" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M47" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N47" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O47" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P47" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>-1</v>
+      </c>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
@@ -3121,12 +3697,24 @@
       <c r="K48" s="3">
         <v>1</v>
       </c>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
+      <c r="L48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>-1</v>
+      </c>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
@@ -3171,12 +3759,24 @@
       <c r="K49" s="3">
         <v>0</v>
       </c>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
+      <c r="L49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>-1</v>
+      </c>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
@@ -3221,12 +3821,24 @@
       <c r="K50" s="3">
         <v>0</v>
       </c>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
+      <c r="L50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>-1</v>
+      </c>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
@@ -3271,12 +3883,24 @@
       <c r="K51" s="3">
         <v>0</v>
       </c>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
+      <c r="L51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>-1</v>
+      </c>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
@@ -3321,12 +3945,24 @@
       <c r="K52" s="3">
         <v>0</v>
       </c>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
+      <c r="L52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>-1</v>
+      </c>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
@@ -3371,12 +4007,24 @@
       <c r="K53" s="3">
         <v>0</v>
       </c>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
+      <c r="L53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>-1</v>
+      </c>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
@@ -3421,12 +4069,24 @@
       <c r="K54" s="3">
         <v>2</v>
       </c>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
+      <c r="L54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>-1</v>
+      </c>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
@@ -3471,12 +4131,24 @@
       <c r="K55" s="3">
         <v>0</v>
       </c>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
+      <c r="L55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>-1</v>
+      </c>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
@@ -3521,12 +4193,24 @@
       <c r="K56" s="3">
         <v>1</v>
       </c>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
+      <c r="L56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>-1</v>
+      </c>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
@@ -3571,12 +4255,24 @@
       <c r="K57" s="3">
         <v>0</v>
       </c>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
+      <c r="L57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q57" s="2">
+        <v>-1</v>
+      </c>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
@@ -3621,12 +4317,24 @@
       <c r="K58" s="3">
         <v>0</v>
       </c>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
+      <c r="L58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q58" s="2">
+        <v>-1</v>
+      </c>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
@@ -3671,12 +4379,24 @@
       <c r="K59" s="3">
         <v>2</v>
       </c>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
+      <c r="L59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>-1</v>
+      </c>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
@@ -3721,12 +4441,24 @@
       <c r="K60" s="3">
         <v>0</v>
       </c>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
+      <c r="L60" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M60" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N60" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O60" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P60" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>-1</v>
+      </c>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
@@ -3771,12 +4503,24 @@
       <c r="K61" s="3">
         <v>1</v>
       </c>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
+      <c r="L61" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M61" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N61" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O61" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P61" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q61" s="2">
+        <v>-1</v>
+      </c>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
@@ -3821,12 +4565,24 @@
       <c r="K62" s="3">
         <v>0</v>
       </c>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
+      <c r="L62" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M62" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N62" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O62" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P62" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>-1</v>
+      </c>
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
@@ -3871,12 +4627,24 @@
       <c r="K63" s="3">
         <v>2</v>
       </c>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
+      <c r="L63" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M63" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N63" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O63" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P63" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q63" s="2">
+        <v>-1</v>
+      </c>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
@@ -3921,12 +4689,24 @@
       <c r="K64" s="3">
         <v>0</v>
       </c>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
+      <c r="L64" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M64" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N64" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O64" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P64" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>-1</v>
+      </c>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
@@ -3971,12 +4751,24 @@
       <c r="K65" s="3">
         <v>0</v>
       </c>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
+      <c r="L65" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M65" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N65" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O65" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P65" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q65" s="2">
+        <v>-1</v>
+      </c>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
@@ -4021,12 +4813,24 @@
       <c r="K66" s="3">
         <v>2</v>
       </c>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
+      <c r="L66" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M66" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N66" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O66" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P66" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q66" s="2">
+        <v>-1</v>
+      </c>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
@@ -4071,12 +4875,24 @@
       <c r="K67" s="3">
         <v>-2</v>
       </c>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
+      <c r="L67" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M67" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N67" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O67" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P67" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q67" s="2">
+        <v>-1</v>
+      </c>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
@@ -4121,12 +4937,24 @@
       <c r="K68" s="3">
         <v>0</v>
       </c>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
+      <c r="L68" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M68" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N68" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O68" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P68" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q68" s="2">
+        <v>-1</v>
+      </c>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
@@ -4171,12 +4999,24 @@
       <c r="K69" s="3">
         <v>0</v>
       </c>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
+      <c r="L69" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M69" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N69" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O69" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P69" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q69" s="2">
+        <v>-1</v>
+      </c>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
@@ -4221,12 +5061,24 @@
       <c r="K70" s="3">
         <v>2</v>
       </c>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
+      <c r="L70" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M70" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N70" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O70" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P70" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q70" s="2">
+        <v>-1</v>
+      </c>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
@@ -4271,12 +5123,24 @@
       <c r="K71" s="3">
         <v>0</v>
       </c>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
+      <c r="L71" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M71" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N71" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O71" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P71" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>-1</v>
+      </c>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
@@ -4321,12 +5185,24 @@
       <c r="K72" s="3">
         <v>4</v>
       </c>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
+      <c r="L72" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M72" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N72" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O72" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P72" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q72" s="2">
+        <v>-1</v>
+      </c>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
@@ -4371,12 +5247,24 @@
       <c r="K73" s="3">
         <v>0</v>
       </c>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
+      <c r="L73" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M73" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N73" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O73" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P73" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q73" s="2">
+        <v>-1</v>
+      </c>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
@@ -4421,12 +5309,24 @@
       <c r="K74" s="3">
         <v>0</v>
       </c>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
+      <c r="L74" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M74" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N74" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O74" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P74" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q74" s="2">
+        <v>-1</v>
+      </c>
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
@@ -4471,12 +5371,24 @@
       <c r="K75" s="3">
         <v>-2</v>
       </c>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
+      <c r="L75" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M75" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N75" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O75" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P75" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q75" s="2">
+        <v>-1</v>
+      </c>
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
@@ -4521,12 +5433,24 @@
       <c r="K76" s="3">
         <v>1</v>
       </c>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
+      <c r="L76" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M76" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N76" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O76" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P76" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q76" s="2">
+        <v>-1</v>
+      </c>
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
@@ -4571,12 +5495,24 @@
       <c r="K77" s="3">
         <v>0</v>
       </c>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
+      <c r="L77" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M77" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N77" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O77" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P77" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q77" s="2">
+        <v>-1</v>
+      </c>
       <c r="R77" s="1"/>
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
@@ -4621,12 +5557,24 @@
       <c r="K78" s="3">
         <v>-3</v>
       </c>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
-      <c r="O78" s="1"/>
-      <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
+      <c r="L78" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M78" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N78" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O78" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P78" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q78" s="2">
+        <v>-1</v>
+      </c>
       <c r="R78" s="1"/>
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
@@ -4671,12 +5619,24 @@
       <c r="K79" s="3">
         <v>0</v>
       </c>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
-      <c r="N79" s="1"/>
-      <c r="O79" s="1"/>
-      <c r="P79" s="1"/>
-      <c r="Q79" s="1"/>
+      <c r="L79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q79" s="2">
+        <v>-1</v>
+      </c>
       <c r="R79" s="1"/>
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
@@ -4721,12 +5681,24 @@
       <c r="K80" s="3">
         <v>1</v>
       </c>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
+      <c r="L80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q80" s="2">
+        <v>-1</v>
+      </c>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
@@ -4771,12 +5743,24 @@
       <c r="K81" s="3">
         <v>0</v>
       </c>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
-      <c r="O81" s="1"/>
-      <c r="P81" s="1"/>
-      <c r="Q81" s="1"/>
+      <c r="L81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q81" s="2">
+        <v>-1</v>
+      </c>
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
@@ -4821,12 +5805,24 @@
       <c r="K82" s="3">
         <v>-1</v>
       </c>
-      <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
-      <c r="N82" s="1"/>
-      <c r="O82" s="1"/>
-      <c r="P82" s="1"/>
-      <c r="Q82" s="1"/>
+      <c r="L82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q82" s="2">
+        <v>-1</v>
+      </c>
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
@@ -4871,12 +5867,24 @@
       <c r="K83" s="3">
         <v>0</v>
       </c>
-      <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
-      <c r="O83" s="1"/>
-      <c r="P83" s="1"/>
-      <c r="Q83" s="1"/>
+      <c r="L83" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M83" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N83" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O83" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P83" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q83" s="2">
+        <v>-1</v>
+      </c>
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
@@ -4921,12 +5929,24 @@
       <c r="K84" s="3">
         <v>0</v>
       </c>
-      <c r="L84" s="1"/>
-      <c r="M84" s="1"/>
-      <c r="N84" s="1"/>
-      <c r="O84" s="1"/>
-      <c r="P84" s="1"/>
-      <c r="Q84" s="1"/>
+      <c r="L84" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M84" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N84" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O84" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P84" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q84" s="2">
+        <v>-1</v>
+      </c>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
@@ -4971,12 +5991,24 @@
       <c r="K85" s="3">
         <v>2</v>
       </c>
-      <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
-      <c r="N85" s="1"/>
-      <c r="O85" s="1"/>
-      <c r="P85" s="1"/>
-      <c r="Q85" s="1"/>
+      <c r="L85" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M85" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N85" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O85" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P85" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q85" s="2">
+        <v>-1</v>
+      </c>
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
@@ -5021,12 +6053,24 @@
       <c r="K86" s="3">
         <v>-2</v>
       </c>
-      <c r="L86" s="1"/>
-      <c r="M86" s="1"/>
-      <c r="N86" s="1"/>
-      <c r="O86" s="1"/>
-      <c r="P86" s="1"/>
-      <c r="Q86" s="1"/>
+      <c r="L86" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M86" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N86" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O86" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P86" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q86" s="2">
+        <v>-1</v>
+      </c>
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
@@ -5071,12 +6115,24 @@
       <c r="K87" s="3">
         <v>1</v>
       </c>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
-      <c r="N87" s="1"/>
-      <c r="O87" s="1"/>
-      <c r="P87" s="1"/>
-      <c r="Q87" s="1"/>
+      <c r="L87" s="2">
+        <v>-1</v>
+      </c>
+      <c r="M87" s="2">
+        <v>-1</v>
+      </c>
+      <c r="N87" s="2">
+        <v>-1</v>
+      </c>
+      <c r="O87" s="2">
+        <v>-1</v>
+      </c>
+      <c r="P87" s="2">
+        <v>-1</v>
+      </c>
+      <c r="Q87" s="2">
+        <v>-1</v>
+      </c>
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
@@ -5099,12 +6155,12 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
-      <c r="L88" s="1"/>
-      <c r="M88" s="1"/>
-      <c r="N88" s="1"/>
-      <c r="O88" s="1"/>
-      <c r="P88" s="1"/>
-      <c r="Q88" s="1"/>
+      <c r="L88" s="2"/>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+      <c r="O88" s="2"/>
+      <c r="P88" s="2"/>
+      <c r="Q88" s="2"/>
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>

</xml_diff>

<commit_message>
start creation of feedback form prefab Remove slider from the top of screen and replace with segmented bar to clearly show changes in satisfaction
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Preston/AllLancashireScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Preston/AllLancashireScenarios.xlsx
@@ -983,8 +983,8 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G138" sqref="G138"/>
+      <pane ySplit="3" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H122" sqref="H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -8360,7 +8360,7 @@
         <v>3</v>
       </c>
       <c r="H120" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I120" s="1">
         <v>4</v>
@@ -8483,10 +8483,18 @@
       <c r="G122" s="1">
         <v>-1</v>
       </c>
-      <c r="H122" s="1"/>
-      <c r="I122" s="1"/>
-      <c r="J122" s="1"/>
-      <c r="K122" s="1"/>
+      <c r="H122" s="1">
+        <v>4</v>
+      </c>
+      <c r="I122" s="1">
+        <v>4</v>
+      </c>
+      <c r="J122" s="1">
+        <v>2</v>
+      </c>
+      <c r="K122" s="1">
+        <v>0</v>
+      </c>
       <c r="L122" s="2">
         <v>-1</v>
       </c>

</xml_diff>

<commit_message>
Compress background music Fixed some translations and UI text not being set Added prevention of duplicate incidents when using the difficulty mapped incidents
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Preston/AllLancashireScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Preston/AllLancashireScenarios.xlsx
@@ -1322,8 +1322,8 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O135" sqref="O135"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="1">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
change converted structure to not contan localization keys
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Preston/AllLancashireScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Preston/AllLancashireScenarios.xlsx
@@ -1322,8 +1322,8 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2804,7 +2804,7 @@
         <v>31</v>
       </c>
       <c r="E25" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F25" s="2">
         <v>4</v>
@@ -2928,7 +2928,7 @@
         <v>33</v>
       </c>
       <c r="E27" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" s="2">
         <v>6</v>
@@ -3238,7 +3238,7 @@
         <v>39</v>
       </c>
       <c r="E32" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2">
         <v>5</v>
@@ -3672,7 +3672,7 @@
         <v>47</v>
       </c>
       <c r="E39" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" s="2">
         <v>7</v>

</xml_diff>